<commit_message>
preparing the loin test cses sheet
preparing the loin test cses sheet
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23004" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,135 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+  <si>
+    <t>SRS ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Test Data</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Project Name:</t>
+  </si>
+  <si>
+    <t>Module Name:</t>
+  </si>
+  <si>
+    <t>Test Designed by:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Designed date: </t>
+  </si>
+  <si>
+    <t>Banking System</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sondos Mahmoud </t>
+  </si>
+  <si>
+    <t>13/5/2019</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precondition </t>
+  </si>
+  <si>
+    <t>1-Open google chrome 
+2- Navigate to URL "      "</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +159,88 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -50,12 +248,108 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,12 +630,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" style="11" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="40.42578125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="19" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+    </row>
+    <row r="6" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" s="16" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="157" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="159" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="160" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="161" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="163" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added coulums of Rewiew
Added coulums of Rewiew
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>SRS ID</t>
   </si>
@@ -145,6 +145,15 @@
   <si>
     <t>1-Open google chrome 
 2- Navigate to URL "      "</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>Review comments</t>
+  </si>
+  <si>
+    <t>priority</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -325,30 +334,29 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J163"/>
+  <dimension ref="A1:K163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -644,13 +652,15 @@
     <col min="4" max="4" width="25.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="40.42578125" style="11" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="19" style="11" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="11"/>
+    <col min="7" max="8" width="21.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="19" style="11" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" style="11" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="11" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -664,7 +674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -678,27 +688,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:10" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-    </row>
-    <row r="6" spans="1:10" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+    <row r="5" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="18" t="s">
         <v>39</v>
       </c>
       <c r="C6" s="10"/>
@@ -708,271 +719,280 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" s="16" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="17"/>
-    </row>
-    <row r="9" spans="1:10" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="J8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+    <row r="12" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
+    <row r="13" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+    <row r="15" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
+    <row r="18" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+    <row r="19" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="82" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="83" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="85" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="86" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="87" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="90" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="91" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="92" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="94" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="95" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="96" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="147" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="148" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="149" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="150" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="151" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="152" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="153" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="154" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="155" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="156" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="157" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="158" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="159" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="160" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="161" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="162" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="163" s="19" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="56" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="58" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="64" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="85" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="95" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="96" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="147" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="148" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="149" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="150" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="151" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="152" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="153" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="154" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="155" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="156" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="157" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="159" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="160" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="161" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="162" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="163" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added from BANK_SYS_TC_Log_R001 to BANK_SYS_TC_Log_R012
added from BANK_SYS_TC_Log_R001 to BANK_SYS_TC_Log_R012
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
   <si>
     <t>SRS ID</t>
   </si>
@@ -154,6 +154,161 @@
   </si>
   <si>
     <t>priority</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Verify that log in page contain  text box with the label "user name"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-approve that the text field is there </t>
+  </si>
+  <si>
+    <t>log in page contain  text box 
+with the label"user name"</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Verify that log in page contain  text box with the label "password"</t>
+  </si>
+  <si>
+    <t>log in page contain  text box 
+with the label"password"</t>
+  </si>
+  <si>
+    <t>Verify that log in page contain  text box with the label "National ID"</t>
+  </si>
+  <si>
+    <t>1-look at the login page 
+            2-approve that the text field is there</t>
+  </si>
+  <si>
+    <t>log in page contain  text box 
+with the label"National ID"</t>
+  </si>
+  <si>
+    <t>Verify that label with the name "login" is a button which is located at the login page</t>
+  </si>
+  <si>
+    <t>1-look at the login page 
+            2-approve that the "login "button is there</t>
+  </si>
+  <si>
+    <t>label with the name "login" is a button which is located at the login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field  accept only characters and numbers  
+</t>
+  </si>
+  <si>
+    <t>user name : sondos33</t>
+  </si>
+  <si>
+    <t>1-Fill  the user name field  with  "user name "
+like in the test data</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name :   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error message "You have entered an invalid format of data, Please try again"
+shall appear 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field dosenot   accept spaces and error message appear 
+</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field dosenot   accept special characters  and error message appear 
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R012</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name : s*)_ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name :sondos  </t>
+  </si>
+  <si>
+    <t>the field Accepts the value 
+ther is no error message 
+appears</t>
+  </si>
+  <si>
+    <t>Verify that user name field  accept numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name :12345567 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field  accept characters with lower case </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field  accept characters with upper case </t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name :SONDOS </t>
+  </si>
+  <si>
+    <t>user name :sondos mahmud 123456789012345678901234567890asd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that User name field  exceeds max length of 32 error message appear </t>
+  </si>
+  <si>
+    <t>1- after exceeding 32 bit the user name field doesnot accept any values</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R013</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R015</t>
+  </si>
+  <si>
+    <t>verify that National ID field accepts only numbers</t>
+  </si>
+  <si>
+    <t>National ID : "2323456tt667"</t>
+  </si>
+  <si>
+    <t>1-Fill  the National ID field  with  "National ID "
+like in the test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field dosenot   accept special characters  and error message appear 
+</t>
+  </si>
+  <si>
+    <t>password: 12345**))__</t>
+  </si>
+  <si>
+    <t>1-Fill  the password field  with  "password "
+like in the test data</t>
   </si>
 </sst>
 </file>
@@ -304,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -357,6 +512,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K163"/>
+  <dimension ref="A1:L167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -650,17 +808,17 @@
     <col min="2" max="2" width="37.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="25.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="40.42578125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" style="11" customWidth="1"/>
-    <col min="7" max="8" width="21.42578125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="19" style="11" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="11"/>
+    <col min="5" max="5" width="46.140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="11" customWidth="1"/>
+    <col min="7" max="9" width="21.42578125" style="11" customWidth="1"/>
+    <col min="10" max="10" width="19" style="11" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="31.85546875" style="11" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -674,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -688,12 +846,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:11" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -703,9 +861,10 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
       <c r="J5" s="20"/>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="K5" s="20"/>
+      <c r="L5" s="13"/>
+    </row>
+    <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>38</v>
       </c>
@@ -720,10 +879,11 @@
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
-      <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:11" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K6" s="10"/>
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:12" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
@@ -749,164 +909,861 @@
         <v>42</v>
       </c>
       <c r="I8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="L8" s="14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="21"/>
+    </row>
+    <row r="10" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="21"/>
+    </row>
+    <row r="11" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="21"/>
+    </row>
+    <row r="12" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+    </row>
+    <row r="13" spans="1:12" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J13" s="21"/>
+    </row>
+    <row r="14" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J14" s="21"/>
+    </row>
+    <row r="15" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="21"/>
+    </row>
+    <row r="16" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" s="21"/>
+    </row>
+    <row r="17" spans="1:10" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+    </row>
+    <row r="19" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="35" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="42" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="44" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="48" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="51" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="53" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="54" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="61" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="63" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="64" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="67" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="68" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="69" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="70" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="73" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="75" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="79" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C19" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+    </row>
+    <row r="20" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+    </row>
+    <row r="21" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J21" s="21"/>
+    </row>
+    <row r="22" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="J22" s="21"/>
+    </row>
+    <row r="23" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+    </row>
+    <row r="24" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+    </row>
+    <row r="25" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+    </row>
+    <row r="26" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+    </row>
+    <row r="27" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+    </row>
+    <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+    </row>
+    <row r="29" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+    </row>
+    <row r="30" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+    </row>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
+    <row r="34" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+    </row>
+    <row r="35" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+    </row>
+    <row r="36" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+    </row>
+    <row r="37" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+    </row>
+    <row r="38" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+    </row>
+    <row r="39" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+    </row>
+    <row r="40" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+    </row>
+    <row r="41" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+    </row>
+    <row r="42" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+    </row>
+    <row r="43" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+    </row>
+    <row r="44" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+    </row>
+    <row r="45" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+    </row>
+    <row r="46" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+    </row>
+    <row r="47" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+    </row>
+    <row r="48" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+    </row>
+    <row r="49" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+    </row>
+    <row r="51" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D51" s="21"/>
+      <c r="E51" s="21"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
+      <c r="J51" s="21"/>
+    </row>
+    <row r="52" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
+      <c r="J52" s="21"/>
+    </row>
+    <row r="53" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+    </row>
+    <row r="54" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="21"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
+      <c r="J54" s="21"/>
+    </row>
+    <row r="55" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="21"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
+      <c r="J55" s="21"/>
+    </row>
+    <row r="56" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="21"/>
+      <c r="E56" s="21"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
+    </row>
+    <row r="58" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+    </row>
+    <row r="59" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+    </row>
+    <row r="60" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="21"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
+      <c r="J60" s="21"/>
+    </row>
+    <row r="61" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="21"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="21"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="21"/>
+    </row>
+    <row r="62" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="21"/>
+    </row>
+    <row r="63" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
+      <c r="J63" s="21"/>
+    </row>
+    <row r="64" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="21"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="21"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
+      <c r="J64" s="21"/>
+    </row>
+    <row r="65" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="21"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="21"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+    </row>
+    <row r="66" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="21"/>
+    </row>
+    <row r="67" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
+      <c r="J67" s="21"/>
+    </row>
+    <row r="68" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+    </row>
+    <row r="69" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+    </row>
+    <row r="70" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+      <c r="F70" s="21"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
+      <c r="J70" s="21"/>
+    </row>
+    <row r="71" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+    </row>
+    <row r="72" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
+      <c r="J72" s="21"/>
+    </row>
+    <row r="73" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="21"/>
+      <c r="E73" s="21"/>
+      <c r="F73" s="21"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
+      <c r="J73" s="21"/>
+    </row>
+    <row r="74" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D74" s="21"/>
+      <c r="E74" s="21"/>
+      <c r="F74" s="21"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
+      <c r="J74" s="21"/>
+    </row>
+    <row r="75" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="82" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -990,9 +1847,13 @@
     <row r="161" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="162" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="163" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="164" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="165" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="167" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B5:K5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added TC related to SRS [BANK_SYS_SRS_Log_R008 ^BANK_SYS_SRS_Log_R009 ^ BANK_SYS_SRS_Log_R010 ^  BANK_SYS_SRS_Log_R011 ]
Added TC related to SRS [BANK_SYS_SRS_Log_R008 ^BANK_SYS_SRS_Log_R009 ^ BANK_SYS_SRS_Log_R010 ^  BANK_SYS_SRS_Log_R011 ]
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
   <si>
     <t>SRS ID</t>
   </si>
@@ -211,17 +211,10 @@
     <t>user name : sondos33</t>
   </si>
   <si>
-    <t>1-Fill  the user name field  with  "user name "
-like in the test data</t>
-  </si>
-  <si>
     <t>High</t>
   </si>
   <si>
     <t>Functional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user name :   </t>
   </si>
   <si>
     <t xml:space="preserve">Error message "You have entered an invalid format of data, Please try again"
@@ -229,15 +222,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user name field dosenot   accept spaces and error message appear 
-</t>
-  </si>
-  <si>
     <t>low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user name field dosenot   accept special characters  and error message appear 
-</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R012</t>
@@ -275,9 +260,6 @@
     <t>user name :sondos mahmud 123456789012345678901234567890asd</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that User name field  exceeds max length of 32 error message appear </t>
-  </si>
-  <si>
     <t>1- after exceeding 32 bit the user name field doesnot accept any values</t>
   </si>
   <si>
@@ -296,19 +278,133 @@
     <t>National ID : "2323456tt667"</t>
   </si>
   <si>
-    <t>1-Fill  the National ID field  with  "National ID "
+    <t xml:space="preserve">Verify that when User name field  exceeds max length of 32 error message appear </t>
+  </si>
+  <si>
+    <t>National ID : "     "</t>
+  </si>
+  <si>
+    <t>National ID : "  123456789123456789**123_34_436   "</t>
+  </si>
+  <si>
+    <t>verify that National ID field doseno accept special characters and error message appear</t>
+  </si>
+  <si>
+    <t>verify that National ID field doseno accept spaces error message appear</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R016</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R017</t>
+  </si>
+  <si>
+    <t>password :
+" Ss12345Mm"</t>
+  </si>
+  <si>
+    <t>password : "12345**))__"</t>
+  </si>
+  <si>
+    <t>user name : "sondos33"
+ 1-password :"123456789Ss"
+2-password : "1111222333Ss"
+3-password : "222233334444Ss"
+4- national ID "12345678912345"</t>
+  </si>
+  <si>
+    <t>the user  account is unavailable for login for the next 24 hours and the user should be notified on his mobile by an SMS that he won't be able to further login on his account for the next 24</t>
+  </si>
+  <si>
+    <t>user name : "sondos33"
+ 1-password :"123456789Ss"
+4- national ID "12345678912345"</t>
+  </si>
+  <si>
+    <t>1-enter  the user name field  with  "user name "
 like in the test data</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that password  field dosenot   accept special characters  and error message appear 
+    <t>1-enter  the National ID field  with  "National ID "
+like in the test data</t>
+  </si>
+  <si>
+    <t>1-enter  the password field  with  "password "
+like in the test data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">after 24 hour of deactivation the
+ account will be activated again and user can log in   </t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R018</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field dose not   accept special characters  and error message appear 
 </t>
   </si>
   <si>
-    <t>password: 12345**))__</t>
-  </si>
-  <si>
-    <t>1-Fill  the password field  with  "password "
-like in the test data</t>
+    <t xml:space="preserve">Verify that password  field  accept
+combination of capital, small character and number to make secure login   
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that when the user enter password wrong more than
+ 3 times, the account to be unavailable for login for the next 24 hours </t>
+  </si>
+  <si>
+    <t>1-enter  the user name field  with  "user name "
+like in the test data
+2- enter wrong password like in "test data"
+3- enter valid National ID like in "test data"
+4-press log in button 
+5- repeat the previous 4 steps for 3 times with different wrong password like in " test data"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that after 24 hour of deactivating the user account because of entering wrong password for 3 times , account will be activated again and user can log in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter  the user name field  with  "user name "
+like in the test data
+2- enter valid password like in "test data"
+3- enter valid National ID like in "test data"
+4-press log in button 
+</t>
+  </si>
+  <si>
+    <t>is there is message tell user it is activated again?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field dose not   accept spaces and error message appear 
+</t>
+  </si>
+  <si>
+    <t>how error message will be shown "pop up window or what?
+The filed related to the error how user will now that the error message is related to that field? Is it will be colored with red?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field dose not   accept special characters  and error message appear 
+</t>
+  </si>
+  <si>
+    <t>verify that Login form  contain register in the form of hyper link</t>
+  </si>
+  <si>
+    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-approve that the hyper link is there
+3- approve that it is clickable  </t>
+  </si>
+  <si>
+    <t>Login form  contain register in the form of hyper link and it is clickable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name : "            "  </t>
   </si>
 </sst>
 </file>
@@ -507,14 +603,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -796,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L167"/>
+  <dimension ref="A1:L171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -807,7 +903,7 @@
     <col min="1" max="1" width="32.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" style="11" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="46.140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" style="11" customWidth="1"/>
     <col min="7" max="9" width="21.42578125" style="11" customWidth="1"/>
@@ -852,16 +948,16 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -921,31 +1017,33 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="15" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J9" s="21"/>
+      <c r="J9" s="19" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -954,24 +1052,24 @@
       <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21" t="s">
+      <c r="D10" s="19"/>
+      <c r="E10" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21" t="s">
+      <c r="G10" s="19"/>
+      <c r="H10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="I10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="21"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
@@ -980,24 +1078,24 @@
       <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21" t="s">
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="I11" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="21"/>
+      <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
@@ -1006,22 +1104,22 @@
       <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21" t="s">
+      <c r="D12" s="19"/>
+      <c r="E12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21" t="s">
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:12" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
@@ -1030,26 +1128,26 @@
       <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21" t="s">
+      <c r="I13" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="I13" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J13" s="21"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
@@ -1058,26 +1156,26 @@
       <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I14" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J14" s="21"/>
+      <c r="D14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="19"/>
     </row>
     <row r="15" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
@@ -1086,26 +1184,26 @@
       <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="21" t="s">
+      <c r="C15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="21"/>
+      <c r="D15" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
@@ -1114,26 +1212,26 @@
       <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I16" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="21"/>
+      <c r="C16" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
@@ -1142,26 +1240,26 @@
       <c r="B17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J17" s="21"/>
+      <c r="C17" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
@@ -1170,598 +1268,733 @@
       <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
+      <c r="C18" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="21" t="s">
+      <c r="C19" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="19"/>
+    </row>
+    <row r="20" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="C20" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J21" s="19"/>
+    </row>
+    <row r="22" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J22" s="19"/>
+    </row>
+    <row r="23" spans="1:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+    </row>
+    <row r="24" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="16" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" s="21" t="s">
+      <c r="B25" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" s="19"/>
+    </row>
+    <row r="27" spans="1:10" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="I27" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="19"/>
+    </row>
+    <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J21" s="21"/>
-    </row>
-    <row r="22" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F22" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="J22" s="21"/>
-    </row>
-    <row r="23" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-    </row>
-    <row r="24" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-    </row>
-    <row r="25" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-    </row>
-    <row r="26" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-    </row>
-    <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="21"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
     </row>
     <row r="31" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
     </row>
     <row r="33" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
     </row>
     <row r="34" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
     </row>
     <row r="36" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
     </row>
     <row r="37" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="21"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
     </row>
     <row r="38" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
     </row>
     <row r="39" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
     </row>
     <row r="40" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
     </row>
     <row r="41" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
     </row>
     <row r="42" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
     </row>
     <row r="43" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
     </row>
     <row r="44" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
     </row>
     <row r="45" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
     </row>
     <row r="46" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
     </row>
     <row r="47" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
     </row>
     <row r="48" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
-      <c r="F48" s="21"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
     </row>
     <row r="49" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="19"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
     </row>
     <row r="50" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
     </row>
     <row r="51" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
     </row>
     <row r="52" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D52" s="21"/>
-      <c r="E52" s="21"/>
-      <c r="F52" s="21"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="19"/>
+      <c r="F52" s="19"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
     </row>
     <row r="53" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
     </row>
     <row r="54" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="21"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
     </row>
     <row r="55" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D55" s="21"/>
-      <c r="E55" s="21"/>
-      <c r="F55" s="21"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="19"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
     </row>
     <row r="56" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D56" s="21"/>
-      <c r="E56" s="21"/>
-      <c r="F56" s="21"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
     </row>
     <row r="57" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
     </row>
     <row r="58" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="21"/>
-      <c r="E58" s="21"/>
-      <c r="F58" s="21"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="19"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
     </row>
     <row r="59" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="21"/>
-      <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="19"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
     </row>
     <row r="60" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="21"/>
-      <c r="E60" s="21"/>
-      <c r="F60" s="21"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="19"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
     </row>
     <row r="61" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D61" s="21"/>
-      <c r="E61" s="21"/>
-      <c r="F61" s="21"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
     </row>
     <row r="62" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="21"/>
-      <c r="E62" s="21"/>
-      <c r="F62" s="21"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="19"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
     </row>
     <row r="63" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
     </row>
     <row r="64" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D64" s="21"/>
-      <c r="E64" s="21"/>
-      <c r="F64" s="21"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="21"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="19"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
     </row>
     <row r="65" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D65" s="21"/>
-      <c r="E65" s="21"/>
-      <c r="F65" s="21"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="19"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
     </row>
     <row r="66" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D66" s="21"/>
-      <c r="E66" s="21"/>
-      <c r="F66" s="21"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="19"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
     </row>
     <row r="67" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D67" s="21"/>
-      <c r="E67" s="21"/>
-      <c r="F67" s="21"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
     </row>
     <row r="68" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
     </row>
     <row r="69" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="F69" s="21"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
-      <c r="J69" s="21"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="19"/>
     </row>
     <row r="70" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
-      <c r="F70" s="21"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
-      <c r="J70" s="21"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+      <c r="I70" s="19"/>
+      <c r="J70" s="19"/>
     </row>
     <row r="71" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
-      <c r="F71" s="21"/>
-      <c r="G71" s="21"/>
-      <c r="H71" s="21"/>
-      <c r="I71" s="21"/>
-      <c r="J71" s="21"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
     </row>
     <row r="72" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="21"/>
-      <c r="J72" s="21"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
     </row>
     <row r="73" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="21"/>
-      <c r="E73" s="21"/>
-      <c r="F73" s="21"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
-      <c r="J73" s="21"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="G73" s="19"/>
+      <c r="H73" s="19"/>
+      <c r="I73" s="19"/>
+      <c r="J73" s="19"/>
     </row>
     <row r="74" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D74" s="21"/>
-      <c r="E74" s="21"/>
-      <c r="F74" s="21"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
-      <c r="J74" s="21"/>
-    </row>
-    <row r="75" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="G74" s="19"/>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+      <c r="J74" s="19"/>
+    </row>
+    <row r="75" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+      <c r="I75" s="19"/>
+      <c r="J75" s="19"/>
+    </row>
+    <row r="76" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="G76" s="19"/>
+      <c r="H76" s="19"/>
+      <c r="I76" s="19"/>
+      <c r="J76" s="19"/>
+    </row>
+    <row r="77" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
+      <c r="I77" s="19"/>
+      <c r="J77" s="19"/>
+    </row>
+    <row r="78" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
+      <c r="H78" s="19"/>
+      <c r="I78" s="19"/>
+      <c r="J78" s="19"/>
+    </row>
     <row r="79" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="80" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1851,6 +2084,10 @@
     <row r="165" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="166" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="167" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="168" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="169" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="170" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="171" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:K5"/>

</xml_diff>

<commit_message>
edited GUI to UI in the field of type
edited GUI to UI in the field of type
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="113">
   <si>
     <t>SRS ID</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>high</t>
-  </si>
-  <si>
-    <t>GUI</t>
   </si>
   <si>
     <t>Verify that log in page contain  text box with the label "password"</t>
@@ -405,6 +402,9 @@
   </si>
   <si>
     <t xml:space="preserve">user name : "            "  </t>
+  </si>
+  <si>
+    <t>UI</t>
   </si>
 </sst>
 </file>
@@ -894,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1039,10 +1039,10 @@
         <v>47</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1053,21 +1053,21 @@
         <v>28</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19" t="s">
         <v>45</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19" t="s">
         <v>47</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="J10" s="19"/>
     </row>
@@ -1079,21 +1079,21 @@
         <v>29</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>52</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>53</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
         <v>47</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="J11" s="19"/>
     </row>
@@ -1105,20 +1105,22 @@
         <v>30</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>56</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="19"/>
+      <c r="I12" s="19" t="s">
+        <v>112</v>
+      </c>
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:12" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1129,23 +1131,23 @@
         <v>31</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>58</v>
-      </c>
       <c r="E13" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="J13" s="19"/>
     </row>
@@ -1157,23 +1159,23 @@
         <v>32</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J14" s="19"/>
     </row>
@@ -1185,23 +1187,23 @@
         <v>33</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>72</v>
-      </c>
       <c r="E15" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J15" s="19"/>
     </row>
@@ -1213,23 +1215,23 @@
         <v>34</v>
       </c>
       <c r="C16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J16" s="19"/>
     </row>
@@ -1241,23 +1243,23 @@
         <v>35</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J17" s="19"/>
     </row>
@@ -1269,23 +1271,23 @@
         <v>36</v>
       </c>
       <c r="C18" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>79</v>
-      </c>
       <c r="E18" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J18" s="19"/>
     </row>
@@ -1297,23 +1299,23 @@
         <v>37</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J19" s="19"/>
     </row>
@@ -1322,26 +1324,26 @@
         <v>22</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J20" s="19"/>
     </row>
@@ -1350,26 +1352,26 @@
         <v>23</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J21" s="19"/>
     </row>
@@ -1378,26 +1380,26 @@
         <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J22" s="19"/>
     </row>
@@ -1406,23 +1408,25 @@
         <v>24</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="F23" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
+      <c r="I23" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="J23" s="19"/>
     </row>
     <row r="24" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1430,25 +1434,27 @@
         <v>24</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C24" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>103</v>
-      </c>
       <c r="F24" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
+      <c r="I24" s="19" t="s">
+        <v>59</v>
+      </c>
       <c r="J24" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="16" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1456,28 +1462,28 @@
         <v>25</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C25" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J25" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1485,26 +1491,26 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J26" s="19"/>
     </row>
@@ -1513,30 +1519,30 @@
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F27" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="J27" s="19"/>
     </row>
     <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>

</xml_diff>

<commit_message>
Added test cases BANK_SYS_TC_Log_R022,BANK_SYS_TC_Log_R023,BANK_SYS_TC_Log_R024 and edited old TCs
Added test cases BANK_SYS_TC_Log_R022,BANK_SYS_TC_Log_R023,BANK_SYS_TC_Log_R024 and edited old TCs
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="138">
   <si>
     <t>SRS ID</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>BANK_SYS_SRS_Log_R009</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Log_R010</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_Log_R011</t>
@@ -159,53 +156,14 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Verify that log in page contain  text box with the label "user name"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-look at the login page 
-            2-approve that the text field is there </t>
-  </si>
-  <si>
-    <t>log in page contain  text box 
-with the label"user name"</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
-    <t>Verify that log in page contain  text box with the label "password"</t>
-  </si>
-  <si>
-    <t>log in page contain  text box 
-with the label"password"</t>
-  </si>
-  <si>
-    <t>Verify that log in page contain  text box with the label "National ID"</t>
-  </si>
-  <si>
-    <t>1-look at the login page 
-            2-approve that the text field is there</t>
-  </si>
-  <si>
-    <t>log in page contain  text box 
-with the label"National ID"</t>
-  </si>
-  <si>
     <t>Verify that label with the name "login" is a button which is located at the login page</t>
-  </si>
-  <si>
-    <t>1-look at the login page 
-            2-approve that the "login "button is there</t>
-  </si>
-  <si>
-    <t>label with the name "login" is a button which is located at the login page</t>
   </si>
   <si>
     <t xml:space="preserve">Verify that user name field  accept only characters and numbers  
 </t>
-  </si>
-  <si>
-    <t>user name : sondos33</t>
   </si>
   <si>
     <t>High</t>
@@ -228,38 +186,15 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">user name : s*)_ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">user name :sondos  </t>
-  </si>
-  <si>
-    <t>the field Accepts the value 
-ther is no error message 
-appears</t>
-  </si>
-  <si>
     <t>Verify that user name field  accept numbers</t>
   </si>
   <si>
-    <t xml:space="preserve">user name :12345567 </t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user name field  accept characters with lower case </t>
   </si>
   <si>
     <t xml:space="preserve">Verify that user name field  accept characters with upper case </t>
   </si>
   <si>
-    <t xml:space="preserve">user name :SONDOS </t>
-  </si>
-  <si>
-    <t>user name :sondos mahmud 123456789012345678901234567890asd</t>
-  </si>
-  <si>
-    <t>1- after exceeding 32 bit the user name field doesnot accept any values</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Log_R013</t>
   </si>
   <si>
@@ -269,38 +204,13 @@
     <t>BANK_SYS_TC_Log_R015</t>
   </si>
   <si>
-    <t>verify that National ID field accepts only numbers</t>
-  </si>
-  <si>
-    <t>National ID : "2323456tt667"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that when User name field  exceeds max length of 32 error message appear </t>
   </si>
   <si>
-    <t>National ID : "     "</t>
-  </si>
-  <si>
-    <t>National ID : "  123456789123456789**123_34_436   "</t>
-  </si>
-  <si>
-    <t>verify that National ID field doseno accept special characters and error message appear</t>
-  </si>
-  <si>
-    <t>verify that National ID field doseno accept spaces error message appear</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Log_R016</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R017</t>
-  </si>
-  <si>
-    <t>password :
-" Ss12345Mm"</t>
-  </si>
-  <si>
-    <t>password : "12345**))__"</t>
   </si>
   <si>
     <t>user name : "sondos33"
@@ -310,43 +220,15 @@
 4- national ID "12345678912345"</t>
   </si>
   <si>
-    <t>the user  account is unavailable for login for the next 24 hours and the user should be notified on his mobile by an SMS that he won't be able to further login on his account for the next 24</t>
-  </si>
-  <si>
     <t>user name : "sondos33"
  1-password :"123456789Ss"
 4- national ID "12345678912345"</t>
   </si>
   <si>
-    <t>1-enter  the user name field  with  "user name "
-like in the test data</t>
-  </si>
-  <si>
-    <t>1-enter  the National ID field  with  "National ID "
-like in the test data</t>
-  </si>
-  <si>
-    <t>1-enter  the password field  with  "password "
-like in the test data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">after 24 hour of deactivation the
- account will be activated again and user can log in   </t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Log_R018</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that password  field dose not   accept special characters  and error message appear 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that password  field  accept
-combination of capital, small character and number to make secure login   
-</t>
   </si>
   <si>
     <t xml:space="preserve">verify that when the user enter password wrong more than
@@ -364,47 +246,313 @@
     <t xml:space="preserve">verify that after 24 hour of deactivating the user account because of entering wrong password for 3 times , account will be activated again and user can log in </t>
   </si>
   <si>
-    <t xml:space="preserve">1-enter  the user name field  with  "user name "
+    <t>is there is message tell user it is activated again?</t>
+  </si>
+  <si>
+    <t>verify that Login form  contain register in the form of hyper link</t>
+  </si>
+  <si>
+    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
+  </si>
+  <si>
+    <t>Login form  contain register in the form of hyper link and it is clickable</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Verify that log in page contains  text box with the label "user name"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-ensure that the hyper link is there
+3- ensure that it is clickable  </t>
+  </si>
+  <si>
+    <t>Verify that log in page contains  text box with the label "password"</t>
+  </si>
+  <si>
+    <t>1-look at the login page 
+            2-ensure that text box with the label "password" exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-look at the login page 
+            2-ensure that text box with the label "user name" exists </t>
+  </si>
+  <si>
+    <t>log in page contains  text box 
+with the label"user name"</t>
+  </si>
+  <si>
+    <t>log in page contains  text box 
+with the label"password"</t>
+  </si>
+  <si>
+    <t>1-look at the login page 
+            2-ensure that text box with the label "National ID" exists</t>
+  </si>
+  <si>
+    <t>log in page contains  text box 
+with the label"National ID"</t>
+  </si>
+  <si>
+    <t>Verify that log in page contains  text box with label "National ID"</t>
+  </si>
+  <si>
+    <t>1-look at the login page 
+            2-ensure that the "login "button exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> login button is located in the login page</t>
+  </si>
+  <si>
+    <t>user name : sondos33
+password:123456789
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t>1-enter  the user name field  with  "user name "
 like in the test data
-2- enter valid password like in "test data"
+2-enter valid password and valid National ID like in test data
+3-press login</t>
+  </si>
+  <si>
+    <t>user name :sondos  
+password:123456789
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t>user name :SONDOS 
+password:123456789
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t>user name :12345567 
+password:123456789
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name :sondos mahmud 123456789012345678901234567890asd
+password:123456789
+National ID:123456789101
+</t>
+  </si>
+  <si>
+    <t>after exceeding 32 bit the user name field doesnot accept any values</t>
+  </si>
+  <si>
+    <t>verify that National ID field accepts numbers</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password: 123456789
+National ID : "2323456tt667"</t>
+  </si>
+  <si>
+    <t>user shall be loged in and redirected to user home page</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password: 123456789
+National ID : "     "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1-enter  valid user name field  with  "user name" like in the test data
+2-enter valid password like in test data
+3-enter  the National ID field  with  "National ID "like in the test data
+4-press login</t>
+  </si>
+  <si>
+    <t>verify that National ID field doseno accept special characters and error message appears</t>
+  </si>
+  <si>
+    <t>verify that National ID field dosenot accept spaces and  error message appears</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password: 123456789
+National ID : "  123456789123456789**123_34_436   "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter  valid user name field  with  "user name" like in the test data
+2-enter valid password like in test data
+3-enter  the National ID field  with like in the test data
+4-press login
+</t>
+  </si>
+  <si>
+    <t>1-enter  valid user name field  with  "user name" like in the test data
+2-enter valid password like in test data
+3-enter  the National ID field  with like in the test data
+4-press login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field dose not   accept special characters to ensure secure login   and error message appear 
+</t>
+  </si>
+  <si>
+    <t>1-enter  valid user name field  with  "user name" like in the test data
+2-enter password like in test data
+3-enter  valid National ID field  with like in the test data
+4-press login</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password : "12345**))__"
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field  accept
+combination of capital, small character and number to make secure login  not less than 8 digits
+</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password :
+" Ss12345Mm"
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field doesnot accept digits  less than 8 digits
+to make secure login
+</t>
+  </si>
+  <si>
+    <t>user name:sondos
+password :
+" Ss123"
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user  account is unavailable for login for the next 24 hours </t>
+  </si>
+  <si>
+    <t>verify that when the user enter password wrong more than
+ 3 times, the user notified on his mobile by an SMS that he won't be able to further login on his account for the next 24</t>
+  </si>
+  <si>
+    <t>user recieves an SMS 
+ on his mobile  that he won't be able to further login on his account for the next 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that when the user enter password wrong for 1 time and then enter the right password he will be loged in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter  the user name field  with valid   "user name "
+like in the test data
+2- enter wrong password like in "test data"
 3- enter valid National ID like in "test data"
 4-press log in button 
+5-enter valid user name ike in "test data"
+6-enter valid password ike in "test data"
+7-enter valid National ID ike in "test data"
+8-press log in </t>
+  </si>
+  <si>
+    <t>user name : "sondos33"
+wrong password: 12As12345
+National ID : 12345678909876
+right password :123Aas12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that when the user enter password wrong for 2 time and then enter the right password he will be loged in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter  the user name field  with valid   "user name "
+like in the test data
+2- enter wrong password like in "test data"
+3- enter valid National ID like in "test data"
+4-press log in button 
+5-repeat the last 4 steps one more time 
+6-enter valid user name ike in "test data"
+7-enter valid password ike in "test data"
+8-enter valid National ID ike in "test data"
+9-press log in </t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>after 24 hour of deactivation the
+ account will be activated again user shall be loged in and redirected to user home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-ensure that 24 hours passed after deactivation
+2-enter valid user name field  with 
+like in the test data
+3- enter valid password like in "test data"
+4- enter valid National ID like in "test data"
+5-press log in button 
 </t>
   </si>
   <si>
-    <t>is there is message tell user it is activated again?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user name field dose not   accept spaces and error message appear 
+    <t>BANK_SYS_SRS_Log_R007
+BANK_SYS_SRS_Log_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R008
+BANK_SYS_SRS_Log_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R020</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R021</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that when user make 
+all fields empty and press 
+log in error message apear </t>
+  </si>
+  <si>
+    <t>1-press login</t>
+  </si>
+  <si>
+    <t>error message shall appear "all fields are mendaory"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that if user try to log in with account is not registered error meassage appear </t>
+  </si>
+  <si>
+    <t xml:space="preserve">in valid account please register as new account </t>
+  </si>
+  <si>
+    <t>1-enter   user name field  with  "user name" like in the test data
+2-enter password like in test data
+3-enter   National ID field  with like in the test data
+4-press login</t>
+  </si>
+  <si>
+    <t>user name:
+password:
+National ID:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that if userenter the 3 fields "user name ","password " ,"National ID"  then he pressed back before he press log in button then he pressed forward the login page appear with empty fields 
 </t>
   </si>
   <si>
-    <t>how error message will be shown "pop up window or what?
-The filed related to the error how user will now that the error message is related to that field? Is it will be colored with red?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify that user name field dose not   accept special characters  and error message appear 
-</t>
-  </si>
-  <si>
-    <t>verify that Login form  contain register in the form of hyper link</t>
-  </si>
-  <si>
-    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-look at the login page 
-            2-approve that the hyper link is there
-3- approve that it is clickable  </t>
-  </si>
-  <si>
-    <t>Login form  contain register in the form of hyper link and it is clickable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user name : "            "  </t>
-  </si>
-  <si>
-    <t>UI</t>
+    <t xml:space="preserve">the login page appear with empty fields </t>
+  </si>
+  <si>
+    <t>1-enter   user name field  with  "user name" like in the test data
+2-enter password like in test data
+3-enter   National ID field  with like in the test data
+4-press back 
+5-press forward</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R023</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R024</t>
   </si>
 </sst>
 </file>
@@ -892,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L171"/>
+  <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -962,10 +1110,10 @@
     </row>
     <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1002,19 +1150,19 @@
         <v>6</v>
       </c>
       <c r="H8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="15" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,27 +1170,27 @@
         <v>16</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1050,24 +1198,24 @@
         <v>17</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="J10" s="19"/>
     </row>
@@ -1076,24 +1224,24 @@
         <v>18</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="J11" s="19"/>
     </row>
@@ -1102,492 +1250,573 @@
         <v>19</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="J12" s="19"/>
     </row>
-    <row r="13" spans="1:12" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J13" s="19"/>
     </row>
-    <row r="14" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J14" s="19"/>
     </row>
-    <row r="15" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J15" s="19"/>
     </row>
-    <row r="16" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J16" s="19"/>
     </row>
-    <row r="17" spans="1:10" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="E17" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="G17" s="19"/>
       <c r="H17" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J17" s="19"/>
     </row>
-    <row r="18" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J18" s="19"/>
     </row>
-    <row r="19" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>22</v>
+    <row r="19" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J19" s="19"/>
     </row>
-    <row r="20" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>22</v>
+    <row r="20" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J20" s="19"/>
     </row>
-    <row r="21" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>23</v>
+    <row r="21" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J21" s="19"/>
     </row>
-    <row r="22" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J22" s="19"/>
     </row>
-    <row r="23" spans="1:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>24</v>
+    <row r="23" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="H23" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="I23" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J23" s="19"/>
     </row>
-    <row r="24" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="F24" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I24" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J24" s="19"/>
+    </row>
+    <row r="25" spans="1:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="19"/>
+    </row>
+    <row r="26" spans="1:10" s="16" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="19" t="s">
         <v>94</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J24" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="16" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="D26" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>60</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
-        <v>61</v>
+        <v>117</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="J26" s="19"/>
     </row>
-    <row r="27" spans="1:10" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="16" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D27" s="19"/>
+        <v>115</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>114</v>
+      </c>
       <c r="E27" s="19" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="G27" s="19"/>
-      <c r="H27" s="19" t="s">
-        <v>58</v>
-      </c>
+      <c r="H27" s="19"/>
       <c r="I27" s="19" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
       <c r="J27" s="19"/>
     </row>
-    <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" s="16" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>67</v>
+      </c>
       <c r="D28" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>118</v>
+      </c>
       <c r="G28" s="19"/>
       <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-    </row>
-    <row r="29" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I28" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>69</v>
+      </c>
       <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="E29" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="H29" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>72</v>
+      </c>
       <c r="J29" s="19"/>
     </row>
-    <row r="30" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+    <row r="30" spans="1:10" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>127</v>
+      </c>
       <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
+      <c r="H30" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="J30" s="19"/>
     </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+    <row r="31" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>130</v>
+      </c>
       <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
+      <c r="H31" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="J31" s="19"/>
     </row>
-    <row r="32" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+    <row r="32" spans="1:10" s="16" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>134</v>
+      </c>
       <c r="G32" s="19"/>
       <c r="H32" s="19"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
     </row>
-    <row r="33" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19"/>
@@ -1596,7 +1825,9 @@
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
     </row>
-    <row r="34" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="19"/>
       <c r="E34" s="19"/>
       <c r="F34" s="19"/>
@@ -1605,7 +1836,9 @@
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
     </row>
-    <row r="35" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="15"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="19"/>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
@@ -1614,7 +1847,9 @@
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
     </row>
-    <row r="36" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
@@ -1623,7 +1858,9 @@
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
     </row>
-    <row r="37" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="15"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="19"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
@@ -1632,7 +1869,9 @@
       <c r="I37" s="19"/>
       <c r="J37" s="19"/>
     </row>
-    <row r="38" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="15"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -1641,7 +1880,8 @@
       <c r="I38" s="19"/>
       <c r="J38" s="19"/>
     </row>
-    <row r="39" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="15"/>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
@@ -1650,7 +1890,8 @@
       <c r="I39" s="19"/>
       <c r="J39" s="19"/>
     </row>
-    <row r="40" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="15"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
@@ -1659,7 +1900,8 @@
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
     </row>
-    <row r="41" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="15"/>
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
@@ -1668,7 +1910,8 @@
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
     </row>
-    <row r="42" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="15"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
@@ -1677,7 +1920,8 @@
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
     </row>
-    <row r="43" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="15"/>
       <c r="D43" s="19"/>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
@@ -1686,7 +1930,8 @@
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
     </row>
-    <row r="44" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="15"/>
       <c r="D44" s="19"/>
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
@@ -1695,7 +1940,8 @@
       <c r="I44" s="19"/>
       <c r="J44" s="19"/>
     </row>
-    <row r="45" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="15"/>
       <c r="D45" s="19"/>
       <c r="E45" s="19"/>
       <c r="F45" s="19"/>
@@ -1704,7 +1950,8 @@
       <c r="I45" s="19"/>
       <c r="J45" s="19"/>
     </row>
-    <row r="46" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="15"/>
       <c r="D46" s="19"/>
       <c r="E46" s="19"/>
       <c r="F46" s="19"/>
@@ -1713,7 +1960,8 @@
       <c r="I46" s="19"/>
       <c r="J46" s="19"/>
     </row>
-    <row r="47" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="15"/>
       <c r="D47" s="19"/>
       <c r="E47" s="19"/>
       <c r="F47" s="19"/>
@@ -1722,7 +1970,8 @@
       <c r="I47" s="19"/>
       <c r="J47" s="19"/>
     </row>
-    <row r="48" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="15"/>
       <c r="D48" s="19"/>
       <c r="E48" s="19"/>
       <c r="F48" s="19"/>
@@ -2001,8 +2250,24 @@
       <c r="I78" s="19"/>
       <c r="J78" s="19"/>
     </row>
-    <row r="79" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="G79" s="19"/>
+      <c r="H79" s="19"/>
+      <c r="I79" s="19"/>
+      <c r="J79" s="19"/>
+    </row>
+    <row r="80" spans="4:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="G80" s="19"/>
+      <c r="H80" s="19"/>
+      <c r="I80" s="19"/>
+      <c r="J80" s="19"/>
+    </row>
     <row r="81" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="82" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2094,6 +2359,8 @@
     <row r="169" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="170" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="171" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="172" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="173" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:K5"/>

</xml_diff>

<commit_message>
Added test case BANK_SYS_TC_Log_R025
Added test case BANK_SYS_TC_Log_R025
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="142">
   <si>
     <t>SRS ID</t>
   </si>
@@ -535,10 +535,6 @@
 National ID:</t>
   </si>
   <si>
-    <t xml:space="preserve">verify that if userenter the 3 fields "user name ","password " ,"National ID"  then he pressed back before he press log in button then he pressed forward the login page appear with empty fields 
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">the login page appear with empty fields </t>
   </si>
   <si>
@@ -553,6 +549,27 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R024</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that if user enter the 3 fields "user name ","password " ,"National ID"  then he pressed back before he press log in button then he pressed forward the login page appear with empty fields 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that if user enter the 3 fields "user name ","password " ,"National ID"  then he pressed log in then the internet disconnected before the home page load 
+after the internet connection back
+he login page appear with empty fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-enter   user name field  with  "user name" like in the test data
+2-enter password like in test data
+3-enter   National ID field  with like in the test
+4-press login and disconnected the internnt at the same time </t>
+  </si>
+  <si>
+    <t>functional</t>
   </si>
 </sst>
 </file>
@@ -1042,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1770,7 +1787,7 @@
     </row>
     <row r="31" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>129</v>
@@ -1795,34 +1812,52 @@
     </row>
     <row r="32" spans="1:10" s="16" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>132</v>
       </c>
       <c r="E32" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="H32" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>141</v>
+      </c>
       <c r="J32" s="19"/>
     </row>
-    <row r="33" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+    <row r="33" spans="2:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>133</v>
+      </c>
       <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="H33" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>141</v>
+      </c>
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added test case BANK_SYS_TC_Log_R026
Added test case BANK_SYS_TC_Log_R026
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="146">
   <si>
     <t>SRS ID</t>
   </si>
@@ -570,6 +570,21 @@
   </si>
   <si>
     <t>functional</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that admin can log in with his registered account </t>
+  </si>
+  <si>
+    <t>1-enter   user name field  with like in the test data
+2-enter password like in test data
+3-enter   National ID field  with like in the test data
+4-press login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin is loged in and admin home page appear </t>
   </si>
 </sst>
 </file>
@@ -1059,8 +1074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1860,12 +1875,22 @@
       </c>
       <c r="J33" s="19"/>
     </row>
-    <row r="34" spans="2:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+    <row r="34" spans="2:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>145</v>
+      </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>

</xml_diff>

<commit_message>
Update Login Test Case
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
   <si>
     <t>SRS ID</t>
   </si>
@@ -141,10 +141,6 @@
   </si>
   <si>
     <t xml:space="preserve">Precondition </t>
-  </si>
-  <si>
-    <t>1-Open google chrome 
-2- Navigate to URL "      "</t>
   </si>
   <si>
     <t>Reviewed By</t>
@@ -260,9 +256,6 @@
     <t>user name :sondos mahmud 123456789012345678901234567890asd</t>
   </si>
   <si>
-    <t>1- after exceeding 32 bit the user name field doesnot accept any values</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_Log_R013</t>
   </si>
   <si>
@@ -275,18 +268,9 @@
     <t>verify that National ID field accepts only numbers</t>
   </si>
   <si>
-    <t>National ID : "2323456tt667"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that when User name field  exceeds max length of 32 error message appear </t>
   </si>
   <si>
-    <t>National ID : "     "</t>
-  </si>
-  <si>
-    <t>National ID : "  123456789123456789**123_34_436   "</t>
-  </si>
-  <si>
     <t>verify that National ID field doseno accept special characters and error message appear</t>
   </si>
   <si>
@@ -299,37 +283,10 @@
     <t>BANK_SYS_TC_Log_R017</t>
   </si>
   <si>
-    <t>password :
-" Ss12345Mm"</t>
-  </si>
-  <si>
-    <t>password : "12345**))__"</t>
-  </si>
-  <si>
-    <t>user name : "sondos33"
- 1-password :"123456789Ss"
-2-password : "1111222333Ss"
-3-password : "222233334444Ss"
-4- national ID "12345678912345"</t>
-  </si>
-  <si>
     <t>the user  account is unavailable for login for the next 24 hours and the user should be notified on his mobile by an SMS that he won't be able to further login on his account for the next 24</t>
   </si>
   <si>
-    <t>user name : "sondos33"
- 1-password :"123456789Ss"
-4- national ID "12345678912345"</t>
-  </si>
-  <si>
     <t>1-enter  the user name field  with  "user name "
-like in the test data</t>
-  </si>
-  <si>
-    <t>1-enter  the National ID field  with  "National ID "
-like in the test data</t>
-  </si>
-  <si>
-    <t>1-enter  the password field  with  "password "
 like in the test data</t>
   </si>
   <si>
@@ -375,25 +332,15 @@
 </t>
   </si>
   <si>
-    <t>is there is message tell user it is activated again?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user name field dose not   accept spaces and error message appear 
 </t>
   </si>
   <si>
-    <t>how error message will be shown "pop up window or what?
-The filed related to the error how user will now that the error message is related to that field? Is it will be colored with red?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user name field dose not   accept special characters  and error message appear 
 </t>
   </si>
   <si>
     <t>verify that Login form  contain register in the form of hyper link</t>
-  </si>
-  <si>
-    <t>there is no test case tells that ustomer cannot login and has accont before registeration</t>
   </si>
   <si>
     <t xml:space="preserve">1-look at the login page 
@@ -404,13 +351,87 @@
     <t>Login form  contain register in the form of hyper link and it is clickable</t>
   </si>
   <si>
-    <t xml:space="preserve">user name : "            "  </t>
+    <t>Bug ID</t>
+  </si>
+  <si>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>after exceeding 32 digits the username field still accepts values</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after exceeding 32 digits the user name field doesnot accept any values</t>
+  </si>
+  <si>
+    <t>BANK_SYS_BUG_Log_001</t>
+  </si>
+  <si>
+    <t>user name : sondos 
+password : Sondos_23
+National ID : "2323456tt667"</t>
+  </si>
+  <si>
+    <t>1- enter valid username  like in test data
+2- enter valid password like in Test data
+3-enter  invalid ID like in Test data  
+4- press on login button</t>
+  </si>
+  <si>
+    <t>user name : sondos 
+password : Sondos_23
+National ID : "     "</t>
+  </si>
+  <si>
+    <t>user name : sondos 
+password : Sondos_23
+National ID : "  123456789123456789**123_34_436   "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name : sondos
+National Id : 12345648978457
+ password : "12345**))__"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name : sondos
+National Id : 12345648978457
+password :
+" Ss12345Mm"
+</t>
+  </si>
+  <si>
+    <t>blocked</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user name : "  alaa gamal          "  </t>
+  </si>
+  <si>
+    <t>BANK_SYS_BUG_Log_002</t>
+  </si>
+  <si>
+    <t>user name : "sondos"
+ 1-password :"123456789Ss"
+2-password : "1111222333Ss"
+3-password : "222233334444Ss"
+4- national ID "12345648978457"</t>
+  </si>
+  <si>
+    <t>user name : "sondos33"
+ 1-password :"123456789Ss"
+4- national ID "12345648978457"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open google chrome 
+2- Navigate to URL </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,7 +521,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -551,11 +572,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -611,6 +667,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -892,10 +960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L171"/>
+  <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -906,15 +974,17 @@
     <col min="4" max="4" width="29.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="46.140625" style="11" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" style="11" customWidth="1"/>
-    <col min="7" max="9" width="21.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" style="11" customWidth="1"/>
+    <col min="8" max="9" width="21.42578125" style="11" customWidth="1"/>
     <col min="10" max="10" width="19" style="11" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" style="11" customWidth="1"/>
     <col min="12" max="12" width="31.85546875" style="11" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="11"/>
+    <col min="13" max="13" width="32.7109375" style="11" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -928,7 +998,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -942,12 +1012,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:12" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
       <c r="C5" s="21"/>
       <c r="D5" s="21"/>
@@ -960,12 +1030,12 @@
       <c r="K5" s="21"/>
       <c r="L5" s="13"/>
     </row>
-    <row r="6" spans="1:12" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -978,8 +1048,8 @@
       <c r="K6" s="10"/>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:14" s="14" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
@@ -1002,22 +1072,26 @@
         <v>6</v>
       </c>
       <c r="H8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="L8" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="15" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="N8" s="24"/>
+    </row>
+    <row r="9" spans="1:14" s="15" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
@@ -1025,27 +1099,30 @@
         <v>27</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="G9" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19" t="s">
+      <c r="I9" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="19" t="s">
-        <v>48</v>
-      </c>
       <c r="J9" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="M9" s="23"/>
+    </row>
+    <row r="10" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
@@ -1053,25 +1130,29 @@
         <v>28</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G10" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>49</v>
+      </c>
       <c r="H10" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="19"/>
-    </row>
-    <row r="11" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
@@ -1079,25 +1160,29 @@
         <v>29</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="19" t="s">
+        <v>52</v>
+      </c>
       <c r="H11" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J11" s="19"/>
-    </row>
-    <row r="12" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
@@ -1105,23 +1190,27 @@
         <v>30</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="19" t="s">
+        <v>55</v>
+      </c>
       <c r="H12" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-    </row>
-    <row r="13" spans="1:12" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
@@ -1129,27 +1218,31 @@
         <v>31</v>
       </c>
       <c r="C13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19" t="s">
+      <c r="I13" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="19"/>
-    </row>
-    <row r="14" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -1157,27 +1250,31 @@
         <v>32</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="H14" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="19"/>
-    </row>
-    <row r="15" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
@@ -1185,27 +1282,31 @@
         <v>33</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>72</v>
-      </c>
       <c r="E15" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="H15" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="19"/>
-    </row>
-    <row r="16" spans="1:12" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
@@ -1213,27 +1314,31 @@
         <v>34</v>
       </c>
       <c r="C16" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G16" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="H16" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I16" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="1:10" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -1241,27 +1346,32 @@
         <v>35</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="G17" s="19"/>
+        <v>102</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="H17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I17" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="19"/>
-    </row>
-    <row r="18" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="M17" s="15"/>
+    </row>
+    <row r="18" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>22</v>
       </c>
@@ -1269,27 +1379,29 @@
         <v>36</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I18" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="19"/>
-    </row>
-    <row r="19" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J18" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>22</v>
       </c>
@@ -1297,246 +1409,266 @@
         <v>37</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" s="19"/>
-    </row>
-    <row r="20" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J19" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="16" customFormat="1" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="19"/>
-    </row>
-    <row r="21" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J20" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" s="19"/>
-    </row>
-    <row r="22" spans="1:10" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J21" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J22" s="19"/>
-    </row>
-    <row r="23" spans="1:10" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J22" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="16" customFormat="1" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-    </row>
-    <row r="24" spans="1:10" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="M23" s="15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="19" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="16" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F25" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="H25" s="19" t="s">
-        <v>62</v>
-      </c>
       <c r="I25" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F26" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="J26" s="19"/>
-    </row>
-    <row r="27" spans="1:10" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+      <c r="J26" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="J27" s="19"/>
-    </row>
-    <row r="28" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="J27" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
@@ -1545,7 +1677,7 @@
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
     </row>
-    <row r="29" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="19"/>
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
@@ -1554,7 +1686,7 @@
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
     </row>
-    <row r="30" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="19"/>
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
@@ -1563,7 +1695,7 @@
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
     </row>
-    <row r="31" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="19"/>
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
@@ -1572,7 +1704,7 @@
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
     </row>
-    <row r="32" spans="1:10" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>

</xml_diff>

<commit_message>
review testcases for the login module
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\testing\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="124">
   <si>
     <t>SRS ID</t>
   </si>
@@ -265,16 +265,7 @@
     <t>BANK_SYS_TC_Log_R015</t>
   </si>
   <si>
-    <t>verify that National ID field accepts only numbers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that when User name field  exceeds max length of 32 error message appear </t>
-  </si>
-  <si>
-    <t>verify that National ID field doseno accept special characters and error message appear</t>
-  </si>
-  <si>
-    <t>verify that National ID field doseno accept spaces error message appear</t>
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R016</t>
@@ -427,11 +418,61 @@
     <t xml:space="preserve">1-Open google chrome 
 2- Navigate to URL </t>
   </si>
+  <si>
+    <t>complete the test data after click
+ on the login button .</t>
+  </si>
+  <si>
+    <t>1- complete the test data after click
+ on the login button .
+2- username field must contains characters and numbers both .</t>
+  </si>
+  <si>
+    <t>verify that National ID field doesn't accept characters.</t>
+  </si>
+  <si>
+    <t>verify that National ID field dosnot accept space.</t>
+  </si>
+  <si>
+    <t>verify that National ID field dosn't accept special characters.</t>
+  </si>
+  <si>
+    <t>1- missing testcases related to boundary value analysis to national id 
+13,14,15</t>
+  </si>
+  <si>
+    <t>1- password accept special 
+characters , refer again to srs.</t>
+  </si>
+  <si>
+    <t>1- title can be clear more than that ,as
+ you write accept and there is an error
+ message in the expected , although in
+ this case error messgae will appear
+ as password doesn't contain special
+ characters.
+2- use the boundary value analysis for the password field 8:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-complete the test data after click
+ on the login button .
+2- use boundary value analysis technique as user name length from 3:32
+</t>
+  </si>
+  <si>
+    <t>1-missing testcase to verify the hyper link 
+functionality , as clicking on it will 
+redirect customer to regiteration form correctly 
+2- missing happy scenario.</t>
+  </si>
+  <si>
+    <t>khadija mostafa</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,7 +652,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -662,12 +703,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -679,6 +714,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -962,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="D24" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9:K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -978,7 +1022,7 @@
     <col min="8" max="9" width="21.42578125" style="11" customWidth="1"/>
     <col min="10" max="10" width="19" style="11" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" style="11" customWidth="1"/>
+    <col min="12" max="12" width="47.28515625" style="11" customWidth="1"/>
     <col min="13" max="13" width="32.7109375" style="11" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="11"/>
   </cols>
@@ -1018,16 +1062,16 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:14" s="12" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:14" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1035,7 +1079,7 @@
         <v>38</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -1083,13 +1127,13 @@
       <c r="K8" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L8" s="22" t="s">
+      <c r="L8" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="N8" s="24"/>
+      <c r="M8" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="N8" s="22"/>
     </row>
     <row r="9" spans="1:14" s="15" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -1118,9 +1162,12 @@
         <v>47</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="M9" s="23"/>
+        <v>96</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M9" s="21"/>
     </row>
     <row r="10" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
@@ -1149,7 +1196,10 @@
         <v>47</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1179,7 +1229,10 @@
         <v>47</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1207,7 +1260,10 @@
       </c>
       <c r="I12" s="19"/>
       <c r="J12" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1224,7 +1280,7 @@
         <v>57</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F13" s="19" t="s">
         <v>66</v>
@@ -1239,10 +1295,16 @@
         <v>59</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="16" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>20</v>
       </c>
@@ -1256,7 +1318,7 @@
         <v>65</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>66</v>
@@ -1271,10 +1333,16 @@
         <v>59</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="16" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
@@ -1288,7 +1356,7 @@
         <v>71</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>66</v>
@@ -1303,10 +1371,16 @@
         <v>59</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L15" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="16" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>20</v>
       </c>
@@ -1320,7 +1394,7 @@
         <v>68</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F16" s="19" t="s">
         <v>66</v>
@@ -1335,10 +1409,16 @@
         <v>59</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L16" s="24" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
@@ -1346,19 +1426,19 @@
         <v>35</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>72</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>61</v>
@@ -1367,7 +1447,13 @@
         <v>59</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>121</v>
       </c>
       <c r="M17" s="15"/>
     </row>
@@ -1379,13 +1465,13 @@
         <v>36</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>60</v>
@@ -1398,7 +1484,10 @@
         <v>59</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1409,13 +1498,13 @@
         <v>37</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F19" s="19" t="s">
         <v>60</v>
@@ -1428,7 +1517,10 @@
         <v>59</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="16" customFormat="1" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1439,13 +1531,13 @@
         <v>62</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>60</v>
@@ -1458,7 +1550,13 @@
         <v>59</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1469,13 +1567,13 @@
         <v>73</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F21" s="19" t="s">
         <v>60</v>
@@ -1488,10 +1586,16 @@
         <v>59</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L21" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="16" customFormat="1" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>23</v>
       </c>
@@ -1499,13 +1603,13 @@
         <v>74</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>60</v>
@@ -1518,7 +1622,13 @@
         <v>59</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="16" customFormat="1" ht="153.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1529,25 +1639,28 @@
         <v>75</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
       <c r="J23" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="M23" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1555,28 +1668,31 @@
         <v>24</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D24" s="19" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F24" s="19" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
       <c r="I24" s="19"/>
       <c r="J24" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>123</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1584,16 +1700,16 @@
         <v>25</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D25" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F25" s="19" t="s">
         <v>60</v>
@@ -1605,7 +1721,10 @@
         <v>59</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:13" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1613,16 +1732,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>64</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F26" s="19" t="s">
         <v>60</v>
@@ -1635,25 +1754,28 @@
         <v>59</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="K26" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D27" s="19"/>
       <c r="E27" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G27" s="19"/>
       <c r="H27" s="19" t="s">
@@ -1663,7 +1785,13 @@
         <v>47</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L27" s="24" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:13" s="16" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Edited test cases ID
Edited test cases ID
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="174">
   <si>
     <t>SRS ID</t>
   </si>
@@ -673,6 +673,24 @@
     <t>user name:ss33rrrrr
 password:sadfSa224
 National ID:3344556677889</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R017</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R029</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R030</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R031</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R033</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1651,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>122</v>
@@ -1661,7 +1679,7 @@
         <v>124</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C21" s="28" t="s">
         <v>123</v>
@@ -1689,7 +1707,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C22" s="28" t="s">
         <v>67</v>
@@ -1717,7 +1735,7 @@
         <v>129</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>126</v>
@@ -1745,7 +1763,7 @@
         <v>81</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C24" s="28" t="s">
         <v>131</v>
@@ -1773,7 +1791,7 @@
         <v>81</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>50</v>
+        <v>168</v>
       </c>
       <c r="C25" s="28" t="s">
         <v>130</v>
@@ -1801,7 +1819,7 @@
         <v>133</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C26" s="28" t="s">
         <v>134</v>
@@ -1829,7 +1847,7 @@
         <v>82</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>136</v>
@@ -1857,7 +1875,7 @@
         <v>82</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>138</v>
@@ -1885,7 +1903,7 @@
         <v>82</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="C29" s="28" t="s">
         <v>154</v>
@@ -1913,7 +1931,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>55</v>
@@ -1941,7 +1959,7 @@
         <v>23</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="C31" s="28" t="s">
         <v>73</v>
@@ -1969,7 +1987,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C32" s="28" t="s">
         <v>75</v>
@@ -1997,7 +2015,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C33" s="28" t="s">
         <v>77</v>
@@ -2025,7 +2043,7 @@
         <v>23</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C34" s="28" t="s">
         <v>159</v>
@@ -2053,7 +2071,7 @@
         <v>23</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C35" s="28" t="s">
         <v>161</v>
@@ -2081,7 +2099,7 @@
         <v>24</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="C36" s="28" t="s">
         <v>57</v>
@@ -2107,7 +2125,7 @@
         <v>165</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="C37" s="28" t="s">
         <v>86</v>
@@ -2132,7 +2150,7 @@
     </row>
     <row r="38" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
-        <v>96</v>
+        <v>170</v>
       </c>
       <c r="C38" s="28" t="s">
         <v>89</v>
@@ -2157,7 +2175,7 @@
     </row>
     <row r="39" spans="1:10" s="12" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="C39" s="28" t="s">
         <v>97</v>
@@ -2182,7 +2200,7 @@
     </row>
     <row r="40" spans="1:10" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>98</v>
@@ -2207,7 +2225,7 @@
     </row>
     <row r="41" spans="1:10" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="C41" s="28" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
adding review comments to login module
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\review sondos\Internet-Banking-System\Testing\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
   <si>
     <t>SRS ID</t>
   </si>
@@ -691,6 +691,57 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R033</t>
+  </si>
+  <si>
+    <t>uncleared description : 
+verify that login page contains login button.</t>
+  </si>
+  <si>
+    <t>happy scenario : verify that user 
+name can login successfully.</t>
+  </si>
+  <si>
+    <t>user name accept characters only 
+or characters and numbers not numbers only ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check test data and steps ad you write
+username in both </t>
+  </si>
+  <si>
+    <t>1- check error message as it will be the 
+length between 3 and 32.
+2- missing test case to check that username doesn't accept special 
+characters.</t>
+  </si>
+  <si>
+    <t>again duplicated with happy scenario.</t>
+  </si>
+  <si>
+    <t>missing test cases related to boundary
+value analysis of length of national id :
+13,14,15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check test data ,it mustnot contain numbers </t>
+  </si>
+  <si>
+    <t>duplicated with : 
+BANK_SYS_TC_Log_R023</t>
+  </si>
+  <si>
+    <t>description can be better than that.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check error messgae in srs 
+</t>
+  </si>
+  <si>
+    <t>1- missing test cases related to the functionality of " register hyper link 
+2- missing test cases related to password length 8:12 using boundary value analysis .
+3- missing test cases that password 
+doesn't accept (charactera and numbers only )(numbers and special characters only )(characters and special characters only )
+4- check test data for admin same as test data used for customer .</t>
   </si>
 </sst>
 </file>
@@ -841,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,6 +982,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1214,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B41"/>
+    <sheetView tabSelected="1" topLeftCell="G41" workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1229,7 +1283,7 @@
     <col min="7" max="9" width="21.42578125" style="7" customWidth="1"/>
     <col min="10" max="10" width="19" style="7" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="31.85546875" style="7" customWidth="1"/>
+    <col min="12" max="12" width="47.28515625" style="7" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
@@ -1424,7 +1478,7 @@
       </c>
       <c r="J11" s="15"/>
     </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="12" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
@@ -1449,6 +1503,9 @@
         <v>58</v>
       </c>
       <c r="J12" s="15"/>
+      <c r="L12" s="32" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
@@ -1477,6 +1534,9 @@
         <v>45</v>
       </c>
       <c r="J13" s="15"/>
+      <c r="L13" s="32" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="14" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1562,7 +1622,7 @@
       </c>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="12" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>114</v>
       </c>
@@ -1589,8 +1649,11 @@
         <v>45</v>
       </c>
       <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="1:10" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L17" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>118</v>
       </c>
@@ -1617,8 +1680,11 @@
         <v>45</v>
       </c>
       <c r="J18" s="15"/>
-    </row>
-    <row r="19" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L18" s="32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>21</v>
       </c>
@@ -1646,7 +1712,7 @@
       </c>
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1740,7 @@
       </c>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="12" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>124</v>
       </c>
@@ -1701,8 +1767,11 @@
         <v>45</v>
       </c>
       <c r="J21" s="15"/>
-    </row>
-    <row r="22" spans="1:10" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L21" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
@@ -1729,8 +1798,11 @@
         <v>45</v>
       </c>
       <c r="J22" s="15"/>
-    </row>
-    <row r="23" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>129</v>
       </c>
@@ -1757,8 +1829,11 @@
         <v>45</v>
       </c>
       <c r="J23" s="15"/>
-    </row>
-    <row r="24" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L23" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>81</v>
       </c>
@@ -1786,7 +1861,7 @@
       </c>
       <c r="J24" s="15"/>
     </row>
-    <row r="25" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>81</v>
       </c>
@@ -1814,7 +1889,7 @@
       </c>
       <c r="J25" s="15"/>
     </row>
-    <row r="26" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>133</v>
       </c>
@@ -1842,7 +1917,7 @@
       </c>
       <c r="J26" s="15"/>
     </row>
-    <row r="27" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>82</v>
       </c>
@@ -1870,7 +1945,7 @@
       </c>
       <c r="J27" s="15"/>
     </row>
-    <row r="28" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>82</v>
       </c>
@@ -1897,8 +1972,11 @@
         <v>45</v>
       </c>
       <c r="J28" s="15"/>
-    </row>
-    <row r="29" spans="1:10" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="12" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>82</v>
       </c>
@@ -1926,7 +2004,7 @@
       </c>
       <c r="J29" s="15"/>
     </row>
-    <row r="30" spans="1:10" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>23</v>
       </c>
@@ -1953,8 +2031,11 @@
         <v>45</v>
       </c>
       <c r="J30" s="15"/>
-    </row>
-    <row r="31" spans="1:10" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L30" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>23</v>
       </c>
@@ -1982,7 +2063,7 @@
       </c>
       <c r="J31" s="15"/>
     </row>
-    <row r="32" spans="1:10" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>23</v>
       </c>
@@ -2009,8 +2090,11 @@
         <v>45</v>
       </c>
       <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:10" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L32" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>23</v>
       </c>
@@ -2037,8 +2121,11 @@
         <v>45</v>
       </c>
       <c r="J33" s="15"/>
-    </row>
-    <row r="34" spans="1:10" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>23</v>
       </c>
@@ -2066,7 +2153,7 @@
       </c>
       <c r="J34" s="15"/>
     </row>
-    <row r="35" spans="1:10" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>23</v>
       </c>
@@ -2094,7 +2181,7 @@
       </c>
       <c r="J35" s="15"/>
     </row>
-    <row r="36" spans="1:10" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>24</v>
       </c>
@@ -2120,7 +2207,7 @@
       </c>
       <c r="J36" s="15"/>
     </row>
-    <row r="37" spans="1:10" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>165</v>
       </c>
@@ -2148,7 +2235,7 @@
       </c>
       <c r="J37" s="15"/>
     </row>
-    <row r="38" spans="1:10" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>170</v>
       </c>
@@ -2172,8 +2259,11 @@
         <v>45</v>
       </c>
       <c r="J38" s="15"/>
-    </row>
-    <row r="39" spans="1:10" s="12" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L38" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="12" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>171</v>
       </c>
@@ -2198,7 +2288,7 @@
       </c>
       <c r="J39" s="15"/>
     </row>
-    <row r="40" spans="1:10" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>172</v>
       </c>
@@ -2223,7 +2313,7 @@
       </c>
       <c r="J40" s="15"/>
     </row>
-    <row r="41" spans="1:10" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="12" customFormat="1" ht="216.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>173</v>
       </c>
@@ -2247,8 +2337,11 @@
         <v>45</v>
       </c>
       <c r="J41" s="15"/>
-    </row>
-    <row r="42" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L41" s="32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
       <c r="C42" s="28"/>
       <c r="D42" s="21"/>
@@ -2259,7 +2352,7 @@
       <c r="I42" s="15"/>
       <c r="J42" s="15"/>
     </row>
-    <row r="43" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
       <c r="C43" s="28"/>
       <c r="D43" s="21"/>
@@ -2270,7 +2363,7 @@
       <c r="I43" s="15"/>
       <c r="J43" s="15"/>
     </row>
-    <row r="44" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="11"/>
       <c r="C44" s="28"/>
       <c r="D44" s="21"/>
@@ -2281,7 +2374,7 @@
       <c r="I44" s="15"/>
       <c r="J44" s="15"/>
     </row>
-    <row r="45" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="C45" s="28"/>
       <c r="D45" s="21"/>
@@ -2292,7 +2385,7 @@
       <c r="I45" s="15"/>
       <c r="J45" s="15"/>
     </row>
-    <row r="46" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
       <c r="C46" s="29"/>
       <c r="D46" s="21"/>
@@ -2303,7 +2396,7 @@
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
     </row>
-    <row r="47" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="C47" s="29"/>
       <c r="D47" s="21"/>
@@ -2314,7 +2407,7 @@
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
-    <row r="48" spans="1:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
       <c r="C48" s="29"/>
       <c r="D48" s="21"/>

</xml_diff>

<commit_message>
edite login TC up on review comments
edite login TC up on review comments
</commit_message>
<xml_diff>
--- a/Testing/Test Cases/Login TC .xlsx
+++ b/Testing/Test Cases/Login TC .xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\review sondos\Internet-Banking-System\Testing\Test Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="207">
   <si>
     <t>SRS ID</t>
   </si>
@@ -92,9 +92,6 @@
     <t>BANK_SYS_SRS_Log_R006</t>
   </si>
   <si>
-    <t>BANK_SYS_SRS_Log_R007</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_Log_R009</t>
   </si>
   <si>
@@ -137,10 +134,6 @@
     <t xml:space="preserve">Precondition </t>
   </si>
   <si>
-    <t>1-Open google chrome 
-2- Navigate to URL "      "</t>
-  </si>
-  <si>
     <t>Reviewed By</t>
   </si>
   <si>
@@ -154,9 +147,6 @@
   </si>
   <si>
     <t>high</t>
-  </si>
-  <si>
-    <t>Verify that label with the name "login" is a button which is located at the login page</t>
   </si>
   <si>
     <t>High</t>
@@ -240,17 +230,7 @@
 3-press login</t>
   </si>
   <si>
-    <t>verify that National ID field accepts numbers</t>
-  </si>
-  <si>
     <t>user shall be loged in and redirected to user home page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-1-enter  valid user name field  with  "user name" like in the test data
-2-enter valid password like in test data
-3-enter  the National ID field  with  "National ID "like in the test data
-4-press login</t>
   </si>
   <si>
     <t>1-enter  valid user name field  with  "user name" like in the test data
@@ -274,9 +254,6 @@
   <si>
     <t>user recieves an SMS 
  on his mobile  that he won't be able to further login on his account for the next 24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verify that when the user enter password wrong for 1 time and then enter the right password he will be loged in </t>
   </si>
   <si>
     <t xml:space="preserve">1-enter  the user name field  with valid   "user name "
@@ -290,9 +267,6 @@
 8-press log in </t>
   </si>
   <si>
-    <t xml:space="preserve">verify that when the user enter password wrong for 2 time and then enter the right password he will be loged in </t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -337,12 +311,6 @@
     <t xml:space="preserve">low </t>
   </si>
   <si>
-    <t xml:space="preserve">verify that if user try to log in with account is not registered error meassage appear </t>
-  </si>
-  <si>
-    <t xml:space="preserve">in valid account please register as new account </t>
-  </si>
-  <si>
     <t>1-enter   user name field  with  "user name" like in the test data
 2-enter password like in test data
 3-enter   National ID field  with like in the test data
@@ -417,10 +385,6 @@
 2-ensure that text box with the label "password" exists</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user name field  accept characters and numbers  
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Verify that user name field  accept numbers and  characters with lower case </t>
   </si>
   <si>
@@ -467,9 +431,6 @@
   <si>
     <t>BANK_SYS_SRS_Log_R006
 BANK_SYS_SRS_Log_R013</t>
-  </si>
-  <si>
-    <t>Error message appear  below user name field   " the maxmum length is 32 " colored with red</t>
   </si>
   <si>
     <t>verify that National ID is mandatory and  error message appears</t>
@@ -549,11 +510,6 @@
     <t xml:space="preserve">user name:sondos33
 password: Ssondos**33
 </t>
-  </si>
-  <si>
-    <t>user name:sondos33
-password: Ssondos**33
-National ID : 12345678909876</t>
   </si>
   <si>
     <t xml:space="preserve">user name :sondos mahmud 123456789012345678901234567890asd
@@ -715,15 +671,9 @@
 characters.</t>
   </si>
   <si>
-    <t>again duplicated with happy scenario.</t>
-  </si>
-  <si>
     <t>missing test cases related to boundary
 value analysis of length of national id :
 13,14,15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check test data ,it mustnot contain numbers </t>
   </si>
   <si>
     <t>duplicated with : 
@@ -742,6 +692,139 @@
 3- missing test cases that password 
 doesn't accept (charactera and numbers only )(numbers and special characters only )(characters and special characters only )
 4- check test data for admin same as test data used for customer .</t>
+  </si>
+  <si>
+    <t>verify that login page contains login button is located at the login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that user  can login successfully.
+</t>
+  </si>
+  <si>
+    <t>combination of  
+only characters 
+and numbers</t>
+  </si>
+  <si>
+    <t>user name : 
+password:Ssondos**33
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1-enter valid password and valid National ID like in test data
+2-press login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user name field doesnot special characters </t>
+  </si>
+  <si>
+    <t>user name :****$$$$$$
+password:Ssondos**33
+National ID:123456789101</t>
+  </si>
+  <si>
+    <t>Error message appear  below user name field   "length between 3 and 32 " colored with red</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Log_R005
+BANK_SYS_SRS_Log_R007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no  login SRS related to 
+that review comment </t>
+  </si>
+  <si>
+    <t>comments of review comment</t>
+  </si>
+  <si>
+    <t>khadeja mostafa</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> check test data ,it mustnot 
+contain numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">there is no numbers already </t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_TC_Log_R023
+is related to 
+notification on his mobile by an SMS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+verify that after entering password wrong for 1 time user can login with the right password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that after entering password wrong for 2 time user can login with the right password </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verify that user cannot login with un regestered account  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open google chrome 
+2- Navigate to URL "      "
+3-use registerd account </t>
+  </si>
+  <si>
+    <t>no thing happen</t>
+  </si>
+  <si>
+    <t>user name : "admin33"
+ password :Sadmin**33
+national ID "22233445534567"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2- no related SRS log in to it </t>
+  </si>
+  <si>
+    <t xml:space="preserve">if admin/user pressed on register hyper link  he will be redirected to registeration page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin/user is redirected to registeration page </t>
+  </si>
+  <si>
+    <t>1- press on  hyper link "register"</t>
+  </si>
+  <si>
+    <t>user name:sondos33
+password :ssss22222
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field doesnot   accept numbers and special characters only and error message appear 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field doesnot   accept character and numbers onlyand error message appear 
+</t>
+  </si>
+  <si>
+    <t>user name:sondos33
+password :****12345
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that password  field doesnot   accept characters and special characters only and error message appear 
+</t>
+  </si>
+  <si>
+    <t>user name:sondos33
+password :****ssddffgg
+National ID : 12345678909876</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R034</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R035</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R036</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R037</t>
   </si>
 </sst>
 </file>
@@ -977,14 +1060,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,15 +1349,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L180"/>
+  <dimension ref="A1:M183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G41" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" topLeftCell="B44" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.85546875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" style="7" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="34.85546875" style="27" customWidth="1"/>
     <col min="4" max="4" width="38.5703125" style="20" customWidth="1"/>
@@ -1282,18 +1365,19 @@
     <col min="6" max="6" width="32.28515625" style="27" customWidth="1"/>
     <col min="7" max="9" width="21.42578125" style="7" customWidth="1"/>
     <col min="10" max="10" width="19" style="7" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="47.28515625" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="7"/>
+    <col min="13" max="13" width="37.140625" style="7" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="25"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="25"/>
     </row>
-    <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1308,7 +1392,7 @@
       </c>
       <c r="F2" s="25"/>
     </row>
-    <row r="3" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
@@ -1323,32 +1407,32 @@
       </c>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="25"/>
       <c r="D4" s="24"/>
       <c r="E4" s="19"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:12" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
+    <row r="5" spans="1:13" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
       <c r="L5" s="9"/>
     </row>
-    <row r="6" spans="1:12" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>37</v>
+        <v>190</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16"/>
@@ -1361,8 +1445,8 @@
       <c r="K6" s="6"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:12" s="10" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="18.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:13" s="10" customFormat="1" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -1385,1009 +1469,1198 @@
         <v>6</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>7</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="11" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="11" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J9" s="15"/>
-    </row>
-    <row r="10" spans="1:12" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D10" s="21"/>
       <c r="E10" s="21" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J10" s="15"/>
-    </row>
-    <row r="11" spans="1:12" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J11" s="15"/>
-    </row>
-    <row r="12" spans="1:12" s="12" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="12" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>43</v>
+        <v>172</v>
       </c>
       <c r="D12" s="21"/>
       <c r="E12" s="21" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J12" s="15"/>
-      <c r="L12" s="32" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>20</v>
+      <c r="K12" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>180</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J13" s="15"/>
-      <c r="L13" s="32" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L13" s="30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J14" s="15"/>
-    </row>
-    <row r="15" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J15" s="15"/>
-    </row>
-    <row r="16" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J16" s="15"/>
-    </row>
-    <row r="17" spans="1:12" s="12" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>149</v>
+        <v>178</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F17" s="28" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="G17" s="15"/>
       <c r="H17" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J17" s="15"/>
-      <c r="L17" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="12" customFormat="1" ht="72.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D18" s="21" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F18" s="28" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="G18" s="15"/>
       <c r="H18" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J18" s="15"/>
-      <c r="L18" s="32" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>21</v>
+      <c r="K18" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L18" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="12" customFormat="1" ht="54.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>108</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>66</v>
+        <v>176</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="G19" s="15"/>
       <c r="H19" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J19" s="15"/>
-    </row>
-    <row r="20" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G20" s="15"/>
       <c r="H20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="J20" s="15"/>
+      <c r="K20" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="15"/>
-    </row>
-    <row r="21" spans="1:12" s="12" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>49</v>
-      </c>
       <c r="C21" s="28" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>125</v>
+        <v>64</v>
       </c>
       <c r="G21" s="15"/>
       <c r="H21" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J21" s="15"/>
-      <c r="L21" s="32" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>22</v>
+      <c r="K21" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="12" customFormat="1" ht="108.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>67</v>
+        <v>113</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J22" s="15"/>
-      <c r="L22" s="12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K22" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L22" s="30" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G23" s="15"/>
       <c r="H23" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J23" s="15"/>
-      <c r="L23" s="32" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="M23" s="30" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G24" s="15"/>
       <c r="H24" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J24" s="15"/>
-    </row>
-    <row r="25" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="G25" s="15"/>
       <c r="H25" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D26" s="21" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="G26" s="15"/>
       <c r="H26" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J26" s="15"/>
-    </row>
-    <row r="27" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C27" s="28" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D27" s="21" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F27" s="28" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G27" s="15"/>
       <c r="H27" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J27" s="15"/>
-    </row>
-    <row r="28" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K27" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C28" s="28" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D28" s="21" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G28" s="15"/>
       <c r="H28" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J28" s="15"/>
-      <c r="L28" s="12" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K28" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L28" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D29" s="21" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F29" s="28" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J29" s="15"/>
-    </row>
-    <row r="30" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>23</v>
+      <c r="K29" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>55</v>
+        <v>199</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>156</v>
+        <v>197</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="G30" s="15"/>
       <c r="H30" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I30" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="J30" s="15"/>
-      <c r="L30" s="32" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>23</v>
+      <c r="K30" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>73</v>
+        <v>198</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="J31" s="15"/>
-    </row>
-    <row r="32" spans="1:12" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>23</v>
+      <c r="K31" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" s="12" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>75</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>75</v>
+        <v>201</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="F32" s="28" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="G32" s="15"/>
       <c r="H32" s="15" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J32" s="15"/>
-      <c r="L32" s="12" t="s">
+      <c r="K32" s="11" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>158</v>
+        <v>53</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="15" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J33" s="15"/>
-      <c r="L33" s="12" t="s">
+      <c r="K33" s="11" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="M33" s="30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>159</v>
+        <v>68</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>160</v>
+        <v>53</v>
       </c>
       <c r="F34" s="28" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="15" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J34" s="15"/>
-    </row>
-    <row r="35" spans="1:12" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>161</v>
+        <v>187</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I35" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="J35" s="15"/>
-    </row>
-    <row r="36" spans="1:12" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="21"/>
+        <v>188</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="E36" s="21" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="F36" s="28" t="s">
-        <v>164</v>
+        <v>64</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="15" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="J36" s="15"/>
-    </row>
-    <row r="37" spans="1:12" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L36" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="12" customFormat="1" ht="150.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>165</v>
+        <v>22</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>86</v>
+        <v>147</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>48</v>
+        <v>145</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
       <c r="F37" s="28" t="s">
-        <v>166</v>
+        <v>64</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="15" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="J37" s="15"/>
-    </row>
-    <row r="38" spans="1:12" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" s="12" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>22</v>
+      </c>
       <c r="B38" s="11" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I38" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="J38" s="15"/>
-      <c r="L38" s="32" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="12" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K38" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>23</v>
+      </c>
       <c r="B39" s="11" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D39" s="21" t="s">
-        <v>162</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D39" s="21"/>
       <c r="E39" s="21" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
       <c r="J39" s="15"/>
-    </row>
-    <row r="40" spans="1:12" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K39" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="12" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>153</v>
+      </c>
       <c r="B40" s="11" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>162</v>
+        <v>45</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="F40" s="28" t="s">
-        <v>92</v>
+        <v>154</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I40" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I40" s="15" t="s">
-        <v>100</v>
-      </c>
       <c r="J40" s="15"/>
-    </row>
-    <row r="41" spans="1:12" s="12" customFormat="1" ht="216.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K40" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="12" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>102</v>
+        <v>189</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="F41" s="28" t="s">
-        <v>104</v>
+        <v>191</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I41" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I41" s="15" t="s">
-        <v>45</v>
-      </c>
       <c r="J41" s="15"/>
-      <c r="L41" s="32" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="28"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="28"/>
+      <c r="K41" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L41" s="30" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="12" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>83</v>
+      </c>
       <c r="G42" s="15"/>
-      <c r="H42" s="15"/>
-      <c r="I42" s="15"/>
+      <c r="H42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="J42" s="15"/>
-    </row>
-    <row r="43" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="28"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="28"/>
+      <c r="K42" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="12" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="28" t="s">
+        <v>83</v>
+      </c>
       <c r="G43" s="15"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15"/>
+      <c r="H43" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="15" t="s">
+        <v>91</v>
+      </c>
       <c r="J43" s="15"/>
-    </row>
-    <row r="44" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="28"/>
+      <c r="K43" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" s="12" customFormat="1" ht="216.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="E44" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>95</v>
+      </c>
       <c r="G44" s="15"/>
-      <c r="H44" s="15"/>
-      <c r="I44" s="15"/>
+      <c r="H44" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="J44" s="15"/>
-    </row>
-    <row r="45" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="28"/>
+      <c r="K44" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="L44" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="M44" s="12" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="C45" s="28" t="s">
+        <v>194</v>
+      </c>
       <c r="D45" s="21"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="28"/>
+      <c r="E45" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F45" s="28" t="s">
+        <v>195</v>
+      </c>
       <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+      <c r="H45" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="J45" s="15"/>
     </row>
-    <row r="46" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
-      <c r="C46" s="29"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="21"/>
       <c r="E46" s="21"/>
       <c r="F46" s="28"/>
@@ -2396,9 +2669,9 @@
       <c r="I46" s="15"/>
       <c r="J46" s="15"/>
     </row>
-    <row r="47" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
-      <c r="C47" s="29"/>
+      <c r="C47" s="28"/>
       <c r="D47" s="21"/>
       <c r="E47" s="21"/>
       <c r="F47" s="28"/>
@@ -2407,9 +2680,9 @@
       <c r="I47" s="15"/>
       <c r="J47" s="15"/>
     </row>
-    <row r="48" spans="1:12" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
-      <c r="C48" s="29"/>
+      <c r="C48" s="28"/>
       <c r="D48" s="21"/>
       <c r="E48" s="21"/>
       <c r="F48" s="28"/>
@@ -2496,6 +2769,7 @@
       <c r="J55" s="15"/>
     </row>
     <row r="56" spans="2:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="11"/>
       <c r="C56" s="29"/>
       <c r="D56" s="21"/>
       <c r="E56" s="21"/>
@@ -2506,6 +2780,7 @@
       <c r="J56" s="15"/>
     </row>
     <row r="57" spans="2:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="11"/>
       <c r="C57" s="29"/>
       <c r="D57" s="21"/>
       <c r="E57" s="21"/>
@@ -2516,6 +2791,7 @@
       <c r="J57" s="15"/>
     </row>
     <row r="58" spans="2:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="11"/>
       <c r="C58" s="29"/>
       <c r="D58" s="21"/>
       <c r="E58" s="21"/>
@@ -2815,23 +3091,35 @@
       <c r="I87" s="15"/>
       <c r="J87" s="15"/>
     </row>
-    <row r="88" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C88" s="29"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="29"/>
-    </row>
-    <row r="89" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D88" s="21"/>
+      <c r="E88" s="21"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+    </row>
+    <row r="89" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C89" s="29"/>
-      <c r="D89" s="22"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="29"/>
-    </row>
-    <row r="90" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D89" s="21"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+    </row>
+    <row r="90" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C90" s="29"/>
-      <c r="D90" s="22"/>
-      <c r="E90" s="22"/>
-      <c r="F90" s="29"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
     </row>
     <row r="91" spans="3:10" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="29"/>
@@ -3372,6 +3660,24 @@
       <c r="D180" s="22"/>
       <c r="E180" s="22"/>
       <c r="F180" s="29"/>
+    </row>
+    <row r="181" spans="3:6" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C181" s="29"/>
+      <c r="D181" s="22"/>
+      <c r="E181" s="22"/>
+      <c r="F181" s="29"/>
+    </row>
+    <row r="182" spans="3:6" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C182" s="29"/>
+      <c r="D182" s="22"/>
+      <c r="E182" s="22"/>
+      <c r="F182" s="29"/>
+    </row>
+    <row r="183" spans="3:6" s="12" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C183" s="29"/>
+      <c r="D183" s="22"/>
+      <c r="E183" s="22"/>
+      <c r="F183" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>